<commit_message>
ajuste de classificação dos instrumentos DPT, PT, TT e TE
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4007,7 +4007,7 @@
     <row r="2" ht="37.5" customHeight="1">
       <c r="B2" s="33" t="inlineStr">
         <is>
-          <t>Análise Crítica de Calibração dos sensores de Temperatura</t>
+          <t>Análise Crítica de Calibração dos Transmissores de Pressão Diferencial</t>
         </is>
       </c>
     </row>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>FIT-1231010T-TT</t>
+          <t>FIT-1231010T-DPT</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25 - ODS - 70 - TEM - 455</t>
+          <t>25 - ODS - 70 - PRE - 494</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4529,15 +4529,8 @@
         <is>
           <r>
             <rPr/>
-            <t xml:space="preserve">( X ) Sim (  ) Não
+            <t xml:space="preserve">(  ) Sim ( X ) Não
 OBSERVAÇÕES:
-</t>
-          </r>
-          <r>
-            <rPr>
-              <b val="1"/>
-            </rPr>
-            <t xml:space="preserve">Novo range e alarmes alterados no computador de vazão
 </t>
           </r>
         </is>
@@ -4622,7 +4615,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>17/11/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>

</xml_diff>

<commit_message>
comparação entre diêmtro e tamanho da haste
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4007,7 +4007,7 @@
     <row r="2" ht="37.5" customHeight="1">
       <c r="B2" s="33" t="inlineStr">
         <is>
-          <t>Análise Crítica de Calibração dos Transmissores de Pressão Diferencial</t>
+          <t>Análise Crítica de Calibração dos Sensores de Temperatura</t>
         </is>
       </c>
     </row>
@@ -4041,7 +4041,7 @@
       </c>
       <c r="C7" s="34" t="inlineStr">
         <is>
-          <t>FPSO FORTE</t>
+          <t>FPSO-FRADE</t>
         </is>
       </c>
       <c r="D7" s="20" t="n"/>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>FIT-1231010T-DPT</t>
+          <t>045-TE-0040</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>Gás Importado</t>
+          <t>Offloading Run 4</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25 - ODS - 70 - PRE - 494</t>
+          <t>25-ODS-37 - TEM - 385</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="C9" s="27" t="inlineStr">
         <is>
-          <t>14/11/2025</t>
+          <t>05/10/2025</t>
         </is>
       </c>
       <c r="D9" s="20" t="n"/>
@@ -4615,7 +4615,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>17/11/2025</t>
+          <t>07/10/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>
@@ -4647,9 +4647,9 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B23:F23"/>
-    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="C9:D9"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B4:I5"/>

</xml_diff>

<commit_message>
ajuste do gui por motor de comparação
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4041,7 +4041,7 @@
       </c>
       <c r="C7" s="34" t="inlineStr">
         <is>
-          <t>FPSO-FRADE</t>
+          <t>FPSO FORTE</t>
         </is>
       </c>
       <c r="D7" s="20" t="n"/>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>045-TE-0040</t>
+          <t>FIT-1231010T-TT</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>Offloading Run 4</t>
+          <t>Gás Importado</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25-ODS-37 - TEM - 385</t>
+          <t>25 - ODS - 70 - TEM - 455</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="C9" s="27" t="inlineStr">
         <is>
-          <t>05/10/2025</t>
+          <t>14/11/2025</t>
         </is>
       </c>
       <c r="D9" s="20" t="n"/>
@@ -4615,7 +4615,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>07/10/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>
@@ -4647,9 +4647,9 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B23:F23"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B4:I5"/>

</xml_diff>

<commit_message>
ajuste do gui por motor de comparação + alteração range e NS
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4529,8 +4529,15 @@
         <is>
           <r>
             <rPr/>
-            <t xml:space="preserve">(  ) Sim ( X ) Não
+            <t xml:space="preserve">( X ) Sim (  ) Não
 OBSERVAÇÕES:
+</t>
+          </r>
+          <r>
+            <rPr>
+              <b val="1"/>
+            </rPr>
+            <t xml:space="preserve">Novo NS alterado no computador de vazão / XML / SFP
 </t>
           </r>
         </is>
@@ -4647,9 +4654,9 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B23:F23"/>
-    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="C9:D9"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B4:I5"/>

</xml_diff>

<commit_message>
Verificação Local + edição/consulta dados no banco
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4041,7 +4041,7 @@
       </c>
       <c r="C7" s="34" t="inlineStr">
         <is>
-          <t>FPSO FORTE</t>
+          <t>FPSO-</t>
         </is>
       </c>
       <c r="D7" s="20" t="n"/>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>FIT-1231010T-TT</t>
+          <t>045-TE-0040</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>Gás Importado</t>
+          <t>Offloading Run 4</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25 - ODS - 70 - TEM - 455</t>
+          <t>25-ODS-37 - TEM - 385</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="C9" s="27" t="inlineStr">
         <is>
-          <t>14/11/2025</t>
+          <t>05/10/2025</t>
         </is>
       </c>
       <c r="D9" s="20" t="n"/>
@@ -4529,15 +4529,8 @@
         <is>
           <r>
             <rPr/>
-            <t xml:space="preserve">( X ) Sim (  ) Não
+            <t xml:space="preserve">(  ) Sim ( X ) Não
 OBSERVAÇÕES:
-</t>
-          </r>
-          <r>
-            <rPr>
-              <b val="1"/>
-            </rPr>
-            <t xml:space="preserve">Novo NS alterado no computador de vazão / XML / SFP
 </t>
           </r>
         </is>
@@ -4622,7 +4615,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>07/10/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>
@@ -4654,9 +4647,9 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B23:F23"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B4:I5"/>

</xml_diff>

<commit_message>
incluso layout da ods
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4007,7 +4007,7 @@
     <row r="2" ht="37.5" customHeight="1">
       <c r="B2" s="33" t="inlineStr">
         <is>
-          <t>Análise Crítica de Calibração dos Sensores de Temperatura</t>
+          <t>Análise Crítica de Calibração dos Transmissores de Pressão Diferencial</t>
         </is>
       </c>
     </row>
@@ -4041,7 +4041,7 @@
       </c>
       <c r="C7" s="34" t="inlineStr">
         <is>
-          <t>FPSO-</t>
+          <t>FPSO FORTE</t>
         </is>
       </c>
       <c r="D7" s="20" t="n"/>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>045-TE-0040</t>
+          <t>FIT-1231010T-DPT</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>Offloading Run 4</t>
+          <t>Gás Importado</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25-ODS-37 - TEM - 385</t>
+          <t>25 - ODS - 70 - PRE - 494</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="C9" s="27" t="inlineStr">
         <is>
-          <t>05/10/2025</t>
+          <t>14/11/2025</t>
         </is>
       </c>
       <c r="D9" s="20" t="n"/>
@@ -4615,7 +4615,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>07/10/2025</t>
+          <t>17/11/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>
@@ -4647,9 +4647,9 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B23:F23"/>
-    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="C9:D9"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B4:I5"/>

</xml_diff>

<commit_message>
correção atualização no banco + mensagem de arquivo aberto
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4007,7 +4007,7 @@
     <row r="2" ht="37.5" customHeight="1">
       <c r="B2" s="33" t="inlineStr">
         <is>
-          <t>Análise Crítica de Calibração dos Transmissores de Pressão Diferencial</t>
+          <t>Análise Crítica de Calibração dos Transmissores de Pressão</t>
         </is>
       </c>
     </row>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>FIT-1231010T-DPT</t>
+          <t>PIT-5412006</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>Gás Importado</t>
+          <t>HP Flare</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25 - ODS - 70 - PRE - 494</t>
+          <t>25-ODS-70 - PRE - 498</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="C9" s="27" t="inlineStr">
         <is>
-          <t>14/11/2025</t>
+          <t>25/11/2025</t>
         </is>
       </c>
       <c r="D9" s="20" t="n"/>
@@ -4529,8 +4529,15 @@
         <is>
           <r>
             <rPr/>
-            <t xml:space="preserve">(  ) Sim ( X ) Não
+            <t xml:space="preserve">( X ) Sim (  ) Não
 OBSERVAÇÕES:
+</t>
+          </r>
+          <r>
+            <rPr>
+              <b val="1"/>
+            </rPr>
+            <t xml:space="preserve">Novo range e alarmes alterados no computador de vazão
 </t>
           </r>
         </is>
@@ -4615,7 +4622,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>17/11/2025</t>
+          <t>27/11/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>
@@ -4647,9 +4654,9 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B14:F14"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B14:F14"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B4:I5"/>

</xml_diff>

<commit_message>
extração erro fiducial/ajuste da extração para funções
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4012,7 +4012,7 @@
     <row r="2" ht="37.5" customHeight="1">
       <c r="B2" s="34" t="inlineStr">
         <is>
-          <t>Análise Crítica de Calibração dos Transmissores de Pressão Diferencial</t>
+          <t>Análise Crítica de Calibração dos Transmissores de Pressão</t>
         </is>
       </c>
     </row>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>FIT-1231010T-DPT</t>
+          <t>FIT-1231010T-PIT</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4072,7 +4072,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>Gás Importado</t>
+          <t>Gás Importado Periodicity: 3 Meses</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4083,7 +4083,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25 - ODS - 70 - PRE - 494</t>
+          <t>25 - ODS - 70 - PRE - 495</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4620,7 +4620,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>17/11/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>

</xml_diff>

<commit_message>
alerta de incerteza/erro fiducial da calibração
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4012,7 +4012,7 @@
     <row r="2" ht="37.5" customHeight="1">
       <c r="B2" s="34" t="inlineStr">
         <is>
-          <t>Análise Crítica de Calibração dos Transmissores de Pressão</t>
+          <t>Análise Crítica de Calibração dos Sensores de Temperatura</t>
         </is>
       </c>
     </row>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>FIT-1231010T-PIT</t>
+          <t>TE-1223016</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4072,7 +4072,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>Gás Importado Periodicity: 3 Meses</t>
+          <t>Óleo Cargo Tanque A</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4083,7 +4083,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25 - ODS - 70 - PRE - 495</t>
+          <t>25-ODS-70 - TEM - 443</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4098,7 +4098,7 @@
       </c>
       <c r="C9" s="26" t="inlineStr">
         <is>
-          <t>14/11/2025</t>
+          <t>07/11/2025</t>
         </is>
       </c>
       <c r="D9" s="20" t="n"/>
@@ -4620,7 +4620,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>12/11/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>
@@ -4652,9 +4652,9 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B23:F23"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B4:I5"/>

</xml_diff>

<commit_message>
inicio da função de extração dos pontos de calibração
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4012,7 +4012,7 @@
     <row r="2" ht="37.5" customHeight="1">
       <c r="B2" s="34" t="inlineStr">
         <is>
-          <t>Análise Crítica de Calibração dos Sensores de Temperatura</t>
+          <t>Análise Crítica de Calibração dos Transmissores de Pressão</t>
         </is>
       </c>
     </row>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>TE-1223016</t>
+          <t>FIT-1231010T-PIT</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4072,7 +4072,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>Óleo Cargo Tanque A</t>
+          <t>Gás Importado</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4083,7 +4083,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25-ODS-70 - TEM - 443</t>
+          <t>25 - ODS - 70 - PRE - 495</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4098,7 +4098,7 @@
       </c>
       <c r="C9" s="26" t="inlineStr">
         <is>
-          <t>07/11/2025</t>
+          <t>14/11/2025</t>
         </is>
       </c>
       <c r="D9" s="20" t="n"/>
@@ -4620,7 +4620,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>12/11/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>

</xml_diff>

<commit_message>
conversao de valores em kpa 85%
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4046,7 +4046,7 @@
       </c>
       <c r="C7" s="35" t="inlineStr">
         <is>
-          <t>FPSO FORTE</t>
+          <t>FPSO FRADE</t>
         </is>
       </c>
       <c r="D7" s="20" t="n"/>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>FIT-1231010T-PIT</t>
+          <t>075-PT-1501</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4072,7 +4072,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>Gás Importado</t>
+          <t>EXPORT GAS 1</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4083,7 +4083,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25 - ODS - 70 - PRE - 495</t>
+          <t>25 - ODS - 37 - PRE - 513</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4098,7 +4098,7 @@
       </c>
       <c r="C9" s="26" t="inlineStr">
         <is>
-          <t>14/11/2025</t>
+          <t>06/12/2025</t>
         </is>
       </c>
       <c r="D9" s="20" t="n"/>
@@ -4620,7 +4620,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>11/12/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>
@@ -4652,9 +4652,9 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B23:F23"/>
-    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="C9:D9"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B4:I5"/>

</xml_diff>

<commit_message>
função de extração de pontos final sem conversão - DPT/TT/TE
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-12225" yWindow="-15450" windowWidth="14400" windowHeight="7275" tabRatio="600" firstSheet="1" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="15420" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="1" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="BASE" sheetId="1" state="hidden" r:id="rId1"/>
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -82,11 +82,6 @@
       <b val="1"/>
       <color rgb="FF008080"/>
       <sz val="13"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="4">
@@ -282,11 +277,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4005,14 +4000,14 @@
     <col width="20.453125" customWidth="1" style="29" min="6" max="6"/>
     <col width="8.1796875" customWidth="1" style="29" min="7" max="7"/>
     <col width="8" customWidth="1" style="29" min="8" max="9"/>
-    <col width="9.1796875" customWidth="1" style="29" min="10" max="16"/>
-    <col width="9.1796875" customWidth="1" style="29" min="17" max="16384"/>
+    <col width="9.1796875" customWidth="1" style="29" min="10" max="17"/>
+    <col width="9.1796875" customWidth="1" style="29" min="18" max="16384"/>
   </cols>
   <sheetData>
     <row r="2" ht="37.5" customHeight="1">
       <c r="B2" s="34" t="inlineStr">
         <is>
-          <t>Análise Crítica de Calibração dos Transmissores de Pressão</t>
+          <t>Análise Crítica de Calibração dos Sensores de Temperatura</t>
         </is>
       </c>
     </row>
@@ -4046,7 +4041,7 @@
       </c>
       <c r="C7" s="35" t="inlineStr">
         <is>
-          <t>FPSO FRADE</t>
+          <t>FPSO FORTE</t>
         </is>
       </c>
       <c r="D7" s="20" t="n"/>
@@ -4057,7 +4052,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>075-PT-1501</t>
+          <t>TE-5412006</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4072,7 +4067,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>EXPORT GAS 1</t>
+          <t>HP Flare</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4083,7 +4078,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25 - ODS - 37 - PRE - 513</t>
+          <t>25-ODS-70 - TEM - 343</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4096,9 +4091,9 @@
           <t>Data de Calibração:</t>
         </is>
       </c>
-      <c r="C9" s="26" t="inlineStr">
-        <is>
-          <t>06/12/2025</t>
+      <c r="C9" s="27" t="inlineStr">
+        <is>
+          <t>05/09/2025</t>
         </is>
       </c>
       <c r="D9" s="20" t="n"/>
@@ -4620,7 +4615,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>11/12/2025</t>
+          <t>09/09/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>
@@ -4628,7 +4623,7 @@
     <row r="41" ht="36" customHeight="1">
       <c r="B41" s="9" t="n"/>
       <c r="C41" s="10" t="n"/>
-      <c r="D41" s="27" t="inlineStr">
+      <c r="D41" s="26" t="inlineStr">
         <is>
           <t>Responsável pela análise</t>
         </is>
@@ -4652,9 +4647,9 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B14:F14"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B14:F14"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B4:I5"/>

</xml_diff>

<commit_message>
função de extração dos pontos ajustada para aplicar a curva de calibração quando dado em mA a pressão
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4007,7 +4007,7 @@
     <row r="2" ht="37.5" customHeight="1">
       <c r="B2" s="34" t="inlineStr">
         <is>
-          <t>Análise Crítica de Calibração dos Sensores de Temperatura</t>
+          <t>Análise Crítica de Calibração dos Transmissores de Pressão</t>
         </is>
       </c>
     </row>
@@ -4041,7 +4041,7 @@
       </c>
       <c r="C7" s="35" t="inlineStr">
         <is>
-          <t>FPSO FORTE</t>
+          <t>FPSO Forte</t>
         </is>
       </c>
       <c r="D7" s="20" t="n"/>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>TE-5412006</t>
+          <t>FIT-1231006-PT</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>HP Flare</t>
+          <t>Export Gas</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25-ODS-70 - TEM - 343</t>
+          <t>25-ODS-70 - PRE - 373</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="C9" s="27" t="inlineStr">
         <is>
-          <t>05/09/2025</t>
+          <t>25/08/2025</t>
         </is>
       </c>
       <c r="D9" s="20" t="n"/>
@@ -4615,7 +4615,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>09/09/2025</t>
+          <t>29/08/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>
@@ -4647,9 +4647,9 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B14:F14"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B14:F14"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B4:I5"/>

</xml_diff>

<commit_message>
ajuste extração de pontos TT - Função final
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4007,7 +4007,7 @@
     <row r="2" ht="37.5" customHeight="1">
       <c r="B2" s="34" t="inlineStr">
         <is>
-          <t>Análise Crítica de Calibração dos Transmissores de Pressão</t>
+          <t>Análise Crítica de Calibração dos Sensores de Temperatura</t>
         </is>
       </c>
     </row>
@@ -4041,7 +4041,7 @@
       </c>
       <c r="C7" s="35" t="inlineStr">
         <is>
-          <t>FPSO Forte</t>
+          <t>FPSO FORTE</t>
         </is>
       </c>
       <c r="D7" s="20" t="n"/>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>FIT-1231006-PT</t>
+          <t>FIT-1231010T-TT</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>Export Gas</t>
+          <t>Gás Importado</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25-ODS-70 - PRE - 373</t>
+          <t>25 - ODS - 70 - TEM - 455</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="C9" s="27" t="inlineStr">
         <is>
-          <t>25/08/2025</t>
+          <t>14/11/2025</t>
         </is>
       </c>
       <c r="D9" s="20" t="n"/>
@@ -4615,7 +4615,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>29/08/2025</t>
+          <t>18/11/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>

</xml_diff>

<commit_message>
versão final com layout ajustado
</commit_message>
<xml_diff>
--- a/TemplateAC.xlsx
+++ b/TemplateAC.xlsx
@@ -4041,7 +4041,7 @@
       </c>
       <c r="C7" s="35" t="inlineStr">
         <is>
-          <t>FPSO FORTE</t>
+          <t>FPSO BRAVO</t>
         </is>
       </c>
       <c r="D7" s="20" t="n"/>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="F7" s="31" t="inlineStr">
         <is>
-          <t>FIT-1231010T-TT</t>
+          <t>TIT-1125-52</t>
         </is>
       </c>
       <c r="G7" s="19" t="n"/>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="C8" s="18" t="inlineStr">
         <is>
-          <t>Gás Importado</t>
+          <t>Separador de Produção Gás</t>
         </is>
       </c>
       <c r="D8" s="20" t="n"/>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="F8" s="18" t="inlineStr">
         <is>
-          <t>25 - ODS - 70 - TEM - 455</t>
+          <t>25 - ODS - 53 - TEM - 391</t>
         </is>
       </c>
       <c r="G8" s="19" t="n"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="C9" s="27" t="inlineStr">
         <is>
-          <t>14/11/2025</t>
+          <t>02/10/2025</t>
         </is>
       </c>
       <c r="D9" s="20" t="n"/>
@@ -4615,7 +4615,7 @@
       <c r="G40" s="15" t="n"/>
       <c r="H40" s="17" t="inlineStr">
         <is>
-          <t>18/11/2025</t>
+          <t>06/10/2025</t>
         </is>
       </c>
       <c r="I40" s="16" t="n"/>
@@ -4647,9 +4647,9 @@
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B23:F23"/>
+    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="D41:E41"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B4:I5"/>

</xml_diff>